<commit_message>
base2 editada de novo
</commit_message>
<xml_diff>
--- a/data/dados2.xlsx
+++ b/data/dados2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Insper Eng Comp 2 Semestre\codesing de apps\22-2a-cd-p1-grupo_rodrigol5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7EAD37-B330-4975-B1F3-9BE64A799DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E58717-C5CD-4A01-9BC0-50D8929EA344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7363,8 +7363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B105" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="C108" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9895,6 +9895,9 @@
       <c r="E126">
         <v>65</v>
       </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -9912,6 +9915,9 @@
       <c r="E127">
         <v>75</v>
       </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -9928,6 +9934,9 @@
       </c>
       <c r="E128">
         <v>33</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>